<commit_message>
Ajout choix du langage dans le doc spécification technique
- Ajout du Choix de langae dans le document des spécifications techniques entre python et C++
</commit_message>
<xml_diff>
--- a/Journal/Rapport - Matthew Flenet.xlsx
+++ b/Journal/Rapport - Matthew Flenet.xlsx
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SFL2\SFL2_ChaineDeFroid\Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EE1442-3FD8-4C78-B6FD-DC14DF49ED11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA08D54-5A5C-41A0-A8B4-F4DB55CD3296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -34,6 +42,9 @@
   </si>
   <si>
     <t>Durée</t>
+  </si>
+  <si>
+    <t>Création de ce document</t>
   </si>
 </sst>
 </file>
@@ -57,8 +68,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFFFF89"/>
+      <sz val="14"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -119,11 +130,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -422,7 +436,7 @@
   <dimension ref="B2:D200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5703125" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -445,89 +459,93 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="B5" s="3">
+        <v>43847</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
@@ -1436,5 +1454,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>